<commit_message>
Add Ending Credit UI Image
</commit_message>
<xml_diff>
--- a/Assets/9. DataBase/CreditDB.xlsx
+++ b/Assets/9. DataBase/CreditDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projects\Utopia\Assets\9. DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\Utopia\Assets\9. DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6399A7-97ED-4168-A9B0-9A8C2A297E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78722F43-9FB1-42BF-8A0F-E5B2CA518EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23355" yWindow="435" windowWidth="22965" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>spriteIdx</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -31,18 +31,6 @@
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bb</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cc</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -816,10 +804,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C152"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -843,35 +831,38 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10000</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
       <c r="B5">
         <v>0</v>
       </c>
@@ -880,6 +871,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
       <c r="B6">
         <v>0</v>
       </c>
@@ -888,6 +882,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
       <c r="B7">
         <v>0</v>
       </c>
@@ -896,6 +893,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
       <c r="B8">
         <v>0</v>
       </c>
@@ -904,6 +904,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
       <c r="B9">
         <v>0</v>
       </c>
@@ -912,6 +915,9 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
       <c r="B10">
         <v>0</v>
       </c>
@@ -920,6 +926,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
       <c r="B11">
         <v>0</v>
       </c>
@@ -928,6 +937,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
       <c r="B12">
         <v>0</v>
       </c>
@@ -936,6 +948,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
       <c r="B13">
         <v>0</v>
       </c>
@@ -944,38 +959,53 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>816815</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>816815</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
       <c r="B18">
         <v>0</v>
       </c>
@@ -983,7 +1013,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
       <c r="B19">
         <v>0</v>
       </c>
@@ -991,23 +1024,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
       <c r="B20">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
       <c r="B21">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
       <c r="B22">
         <v>0</v>
       </c>
@@ -1015,23 +1057,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
       <c r="B23">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
       <c r="B24">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
       <c r="B25">
         <v>0</v>
       </c>
@@ -1039,15 +1090,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
       <c r="B26">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
       <c r="B27">
         <v>0</v>
       </c>
@@ -1055,7 +1112,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
       <c r="B28">
         <v>0</v>
       </c>
@@ -1063,7 +1123,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
       <c r="B29">
         <v>0</v>
       </c>
@@ -1071,7 +1134,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
       <c r="B30">
         <v>0</v>
       </c>
@@ -1079,7 +1145,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
       <c r="B31">
         <v>0</v>
       </c>
@@ -1087,7 +1156,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
       <c r="B32">
         <v>0</v>
       </c>
@@ -1095,15 +1167,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
       <c r="B33">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
       <c r="B34">
         <v>0</v>
       </c>
@@ -1111,23 +1189,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
       <c r="B35">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>25000</v>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
       </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
       <c r="B37">
         <v>0</v>
       </c>
@@ -1135,23 +1222,32 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
       <c r="B38">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
         <v>0</v>
       </c>
       <c r="C39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
       <c r="B40">
         <v>0</v>
       </c>
@@ -1159,15 +1255,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
       <c r="B41">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
       <c r="B42">
         <v>0</v>
       </c>
@@ -1175,7 +1277,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
       <c r="B43">
         <v>0</v>
       </c>
@@ -1183,7 +1288,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
       <c r="B44">
         <v>0</v>
       </c>
@@ -1191,7 +1299,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
       <c r="B45">
         <v>0</v>
       </c>
@@ -1199,7 +1310,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
       <c r="B46">
         <v>0</v>
       </c>
@@ -1207,7 +1321,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
       <c r="B47">
         <v>0</v>
       </c>
@@ -1215,7 +1332,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
       <c r="B48">
         <v>0</v>
       </c>
@@ -1223,7 +1343,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
       <c r="B49">
         <v>0</v>
       </c>
@@ -1231,7 +1354,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
       <c r="B50">
         <v>0</v>
       </c>
@@ -1239,7 +1365,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
       <c r="B51">
         <v>0</v>
       </c>
@@ -1247,7 +1376,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
       <c r="B52">
         <v>0</v>
       </c>
@@ -1255,7 +1387,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
       <c r="B53">
         <v>0</v>
       </c>
@@ -1263,7 +1398,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
       <c r="B54">
         <v>0</v>
       </c>
@@ -1271,15 +1409,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
       <c r="B55">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
       <c r="B56">
         <v>0</v>
       </c>
@@ -1287,7 +1431,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
       <c r="B57">
         <v>0</v>
       </c>
@@ -1295,15 +1442,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
       <c r="B58">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C58" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
       <c r="B59">
         <v>0</v>
       </c>
@@ -1311,7 +1464,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
       <c r="B60">
         <v>0</v>
       </c>
@@ -1319,15 +1475,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
       <c r="B61">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C61" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
       <c r="B62">
         <v>0</v>
       </c>
@@ -1335,7 +1497,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
       <c r="B63">
         <v>0</v>
       </c>
@@ -1343,7 +1508,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
       <c r="B64">
         <v>50000</v>
       </c>
@@ -1351,15 +1519,21 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
       <c r="B65">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C65" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
       <c r="B66">
         <v>0</v>
       </c>
@@ -1367,23 +1541,32 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
       <c r="B67">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C67" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
       <c r="B68">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="C68" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
       <c r="B69">
         <v>0</v>
       </c>
@@ -1391,7 +1574,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0</v>
+      </c>
       <c r="B70">
         <v>0</v>
       </c>
@@ -1399,15 +1585,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
       <c r="B71">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C71" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
       <c r="B72">
         <v>0</v>
       </c>
@@ -1415,7 +1607,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
       <c r="B73">
         <v>0</v>
       </c>
@@ -1423,7 +1618,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
       <c r="B74">
         <v>0</v>
       </c>
@@ -1431,7 +1629,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
       <c r="B75">
         <v>0</v>
       </c>
@@ -1439,15 +1640,21 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
       <c r="B76">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="C76" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
       <c r="B77">
         <v>0</v>
       </c>
@@ -1455,7 +1662,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
       <c r="B78">
         <v>0</v>
       </c>
@@ -1463,15 +1673,21 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
       <c r="B79">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C79" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0</v>
+      </c>
       <c r="B80">
         <v>0</v>
       </c>
@@ -1479,7 +1695,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
       <c r="B81">
         <v>0</v>
       </c>
@@ -1487,15 +1706,21 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
       <c r="B82">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="C82" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
       <c r="B83">
         <v>0</v>
       </c>
@@ -1503,23 +1728,32 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
       <c r="B84">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="C84" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
       <c r="B85">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C85" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0</v>
+      </c>
       <c r="B86">
         <v>0</v>
       </c>
@@ -1527,15 +1761,21 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
       <c r="B87">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C87" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0</v>
+      </c>
       <c r="B88">
         <v>0</v>
       </c>
@@ -1543,7 +1783,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
       <c r="B89">
         <v>0</v>
       </c>
@@ -1551,7 +1794,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
       <c r="B90">
         <v>0</v>
       </c>
@@ -1559,7 +1805,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
       <c r="B91">
         <v>0</v>
       </c>
@@ -1567,7 +1816,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
       <c r="B92">
         <v>0</v>
       </c>
@@ -1575,7 +1827,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
       <c r="B93">
         <v>0</v>
       </c>
@@ -1583,7 +1838,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0</v>
+      </c>
       <c r="B94">
         <v>0</v>
       </c>
@@ -1591,7 +1849,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
       <c r="B95">
         <v>0</v>
       </c>
@@ -1599,7 +1860,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
       <c r="B96">
         <v>0</v>
       </c>
@@ -1607,7 +1871,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
       <c r="B97">
         <v>0</v>
       </c>
@@ -1615,7 +1882,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
       <c r="B98">
         <v>0</v>
       </c>
@@ -1623,7 +1893,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0</v>
+      </c>
       <c r="B99">
         <v>0</v>
       </c>
@@ -1631,7 +1904,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0</v>
+      </c>
       <c r="B100">
         <v>0</v>
       </c>
@@ -1639,23 +1915,32 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
       <c r="B101">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C101" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102" s="2">
         <v>0</v>
       </c>
       <c r="C102" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>0</v>
+      </c>
       <c r="B103">
         <v>0</v>
       </c>
@@ -1663,23 +1948,32 @@
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>0</v>
+      </c>
       <c r="B104">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C104" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" s="2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>0</v>
+      </c>
+      <c r="B105">
         <v>0</v>
       </c>
       <c r="C105" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>0</v>
+      </c>
       <c r="B106">
         <v>0</v>
       </c>
@@ -1687,7 +1981,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>0</v>
+      </c>
       <c r="B107">
         <v>0</v>
       </c>
@@ -1695,7 +1992,10 @@
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>0</v>
+      </c>
       <c r="B108">
         <v>0</v>
       </c>
@@ -1703,7 +2003,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>0</v>
+      </c>
       <c r="B109">
         <v>0</v>
       </c>
@@ -1711,47 +2014,65 @@
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>0</v>
+      </c>
       <c r="B110">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="C110" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>0</v>
+      </c>
       <c r="B111">
         <v>0</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>0</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112">
-        <v>0</v>
-      </c>
-      <c r="C112" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113">
-        <v>100000</v>
-      </c>
-      <c r="C113" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>0</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114">
-        <v>0</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>0</v>
+      </c>
       <c r="B115">
         <v>0</v>
       </c>
@@ -1759,7 +2080,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0</v>
+      </c>
       <c r="B116">
         <v>0</v>
       </c>
@@ -1767,7 +2091,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>0</v>
+      </c>
       <c r="B117">
         <v>0</v>
       </c>
@@ -1775,7 +2102,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>0</v>
+      </c>
       <c r="B118">
         <v>0</v>
       </c>
@@ -1783,7 +2113,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>0</v>
+      </c>
       <c r="B119">
         <v>0</v>
       </c>
@@ -1791,7 +2124,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>0</v>
+      </c>
       <c r="B120">
         <v>0</v>
       </c>
@@ -1799,63 +2135,87 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>0</v>
+      </c>
       <c r="B121">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="C121" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>0</v>
+      </c>
       <c r="B122">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="C122" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>0</v>
+      </c>
       <c r="B123">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C123" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>0</v>
+      </c>
       <c r="B124">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="C124" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>0</v>
+      </c>
       <c r="B125">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="C125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>0</v>
+      </c>
       <c r="B126">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>0</v>
+      </c>
       <c r="B127">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="C127" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>0</v>
+      </c>
       <c r="B128">
         <v>0</v>
       </c>
@@ -1863,7 +2223,10 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>0</v>
+      </c>
       <c r="B129">
         <v>0</v>
       </c>
@@ -1871,15 +2234,21 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>0</v>
+      </c>
       <c r="B130">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C130" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>0</v>
+      </c>
       <c r="B131">
         <v>0</v>
       </c>
@@ -1887,7 +2256,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>0</v>
+      </c>
       <c r="B132">
         <v>0</v>
       </c>
@@ -1895,7 +2267,10 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>0</v>
+      </c>
       <c r="B133">
         <v>0</v>
       </c>
@@ -1903,23 +2278,32 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>0</v>
+      </c>
       <c r="B134">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="C134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>0</v>
+      </c>
       <c r="B135">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="C135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>0</v>
+      </c>
       <c r="B136">
         <v>0</v>
       </c>
@@ -1927,23 +2311,32 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>0</v>
+      </c>
       <c r="B137">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>0</v>
+      </c>
       <c r="B138">
-        <v>25000</v>
+        <v>100000</v>
       </c>
       <c r="C138" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>0</v>
+      </c>
       <c r="B139">
         <v>0</v>
       </c>
@@ -1951,7 +2344,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>0</v>
+      </c>
       <c r="B140">
         <v>0</v>
       </c>
@@ -1959,15 +2355,21 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>0</v>
+      </c>
       <c r="B141">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>0</v>
+      </c>
       <c r="B142">
         <v>0</v>
       </c>
@@ -1975,7 +2377,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>0</v>
+      </c>
       <c r="B143">
         <v>0</v>
       </c>
@@ -1983,7 +2388,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>0</v>
+      </c>
       <c r="B144">
         <v>0</v>
       </c>
@@ -1991,7 +2399,10 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>0</v>
+      </c>
       <c r="B145">
         <v>0</v>
       </c>
@@ -1999,7 +2410,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>0</v>
+      </c>
       <c r="B146">
         <v>0</v>
       </c>
@@ -2007,7 +2421,10 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>0</v>
+      </c>
       <c r="B147">
         <v>0</v>
       </c>
@@ -2015,7 +2432,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>0</v>
+      </c>
       <c r="B148">
         <v>0</v>
       </c>
@@ -2023,36 +2443,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>0</v>
+      </c>
       <c r="B149">
         <v>0</v>
       </c>
-      <c r="C149" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B150">
-        <v>0</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="C149" s="1" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B151">
-        <v>0</v>
-      </c>
-      <c r="C151" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B152">
-        <v>0</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>